<commit_message>
atualizando relatorio 2 com as metricas para >50k
</commit_message>
<xml_diff>
--- a/Exercicio 2/DTPeformance.xlsx
+++ b/Exercicio 2/DTPeformance.xlsx
@@ -426,16 +426,16 @@
         <v>30</v>
       </c>
       <c r="D2">
-        <v>0.8105420188960716</v>
+        <v>0.8204873197414222</v>
       </c>
       <c r="E2">
-        <v>0.8782725441933319</v>
+        <v>0.654796511627907</v>
       </c>
       <c r="F2">
-        <v>0.8675950486295314</v>
+        <v>0.5970841616964877</v>
       </c>
       <c r="G2">
-        <v>0.8729011453352609</v>
+        <v>0.6246100519930675</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -449,16 +449,16 @@
         <v>30</v>
       </c>
       <c r="D3">
-        <v>0.8123653240510526</v>
+        <v>0.8183325045582629</v>
       </c>
       <c r="E3">
-        <v>0.8768888888888889</v>
+        <v>0.6495293265749457</v>
       </c>
       <c r="F3">
-        <v>0.872236958443855</v>
+        <v>0.5944333996023857</v>
       </c>
       <c r="G3">
-        <v>0.8745567375886526</v>
+        <v>0.6207612456747404</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -472,16 +472,16 @@
         <v>30</v>
       </c>
       <c r="D4">
-        <v>0.8093817337974474</v>
+        <v>0.8186640145864412</v>
       </c>
       <c r="E4">
-        <v>0.8760588497547926</v>
+        <v>0.6493880489560835</v>
       </c>
       <c r="F4">
-        <v>0.8687002652519894</v>
+        <v>0.5977468522200132</v>
       </c>
       <c r="G4">
-        <v>0.8723640399556049</v>
+        <v>0.6224982746721877</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -495,16 +495,16 @@
         <v>30</v>
       </c>
       <c r="D5">
-        <v>0.8093817337974474</v>
+        <v>0.8211503397977788</v>
       </c>
       <c r="E5">
-        <v>0.8768990169794459</v>
+        <v>0.657856093979442</v>
       </c>
       <c r="F5">
-        <v>0.8675950486295314</v>
+        <v>0.5937707090788602</v>
       </c>
       <c r="G5">
-        <v>0.8722222222222222</v>
+        <v>0.6241727621037966</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -518,16 +518,16 @@
         <v>30</v>
       </c>
       <c r="D6">
-        <v>0.8113707939665175</v>
+        <v>0.8188297696005304</v>
       </c>
       <c r="E6">
-        <v>0.877564674397859</v>
+        <v>0.6509433962264151</v>
       </c>
       <c r="F6">
-        <v>0.8698054818744474</v>
+        <v>0.5944333996023857</v>
       </c>
       <c r="G6">
-        <v>0.8736678507992895</v>
+        <v>0.6214063041219258</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -541,16 +541,16 @@
         <v>30</v>
       </c>
       <c r="D7">
-        <v>0.8128625890933201</v>
+        <v>0.8206530747555113</v>
       </c>
       <c r="E7">
-        <v>0.8774738714698688</v>
+        <v>0.6554989075018208</v>
       </c>
       <c r="F7">
-        <v>0.872236958443855</v>
+        <v>0.5964214711729622</v>
       </c>
       <c r="G7">
-        <v>0.8748475778738498</v>
+        <v>0.6245662734212353</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -564,16 +564,16 @@
         <v>30</v>
       </c>
       <c r="D8">
-        <v>0.8093817337974474</v>
+        <v>0.8183325045582629</v>
       </c>
       <c r="E8">
-        <v>0.8774049217002237</v>
+        <v>0.6504005826656956</v>
       </c>
       <c r="F8">
-        <v>0.8669319186560566</v>
+        <v>0.5917826375082836</v>
       </c>
       <c r="G8">
-        <v>0.8721369802090282</v>
+        <v>0.61970853573907</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -587,16 +587,16 @@
         <v>30</v>
       </c>
       <c r="D9">
-        <v>0.8112050389524283</v>
+        <v>0.8196585446709763</v>
       </c>
       <c r="E9">
-        <v>0.8772008023178069</v>
+        <v>0.6530909090909091</v>
       </c>
       <c r="F9">
-        <v>0.870026525198939</v>
+        <v>0.5950960901259112</v>
       </c>
       <c r="G9">
-        <v>0.8735989346354457</v>
+        <v>0.6227461858529819</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -610,16 +610,16 @@
         <v>30</v>
       </c>
       <c r="D10">
-        <v>0.8087187137410907</v>
+        <v>0.8196585446709763</v>
       </c>
       <c r="E10">
-        <v>0.8761160714285714</v>
+        <v>0.6517664023071377</v>
       </c>
       <c r="F10">
-        <v>0.8675950486295314</v>
+        <v>0.5990722332670643</v>
       </c>
       <c r="G10">
-        <v>0.8718347401155042</v>
+        <v>0.6243093922651933</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -633,16 +633,16 @@
         <v>30</v>
       </c>
       <c r="D11">
-        <v>0.8123653240510526</v>
+        <v>0.8196585446709763</v>
       </c>
       <c r="E11">
-        <v>0.8789097408400357</v>
+        <v>0.6517664023071377</v>
       </c>
       <c r="F11">
-        <v>0.8695844385499558</v>
+        <v>0.5990722332670643</v>
       </c>
       <c r="G11">
-        <v>0.8742222222222222</v>
+        <v>0.6243093922651933</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -656,16 +656,16 @@
         <v>30</v>
       </c>
       <c r="D12">
-        <v>0.8092159787833582</v>
+        <v>0.8199900546991546</v>
       </c>
       <c r="E12">
-        <v>0.8767031494304222</v>
+        <v>0.653372008701958</v>
       </c>
       <c r="F12">
-        <v>0.8675950486295314</v>
+        <v>0.5970841616964877</v>
       </c>
       <c r="G12">
-        <v>0.8721253194089545</v>
+        <v>0.6239612188365651</v>
       </c>
     </row>
   </sheetData>

</xml_diff>